<commit_message>
COMPLETE INTERFACING PLEASE CHECK
</commit_message>
<xml_diff>
--- a/documents/projects_and_modules.xlsx
+++ b/documents/projects_and_modules.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -303,8 +303,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,12 +319,24 @@
       <charset val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -339,14 +351,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,7 +421,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -439,10 +453,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -474,7 +487,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -650,14 +662,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -669,7 +681,7 @@
     <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1">
         <v>8051</v>
       </c>
@@ -680,180 +692,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="1" t="s">
         <v>92</v>
       </c>
@@ -865,21 +914,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>8051</v>
@@ -891,22 +940,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -917,21 +966,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="43.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>8051</v>
@@ -943,182 +992,182 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -1129,19 +1178,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>8051</v>
@@ -1153,47 +1202,47 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -1204,19 +1253,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>8051</v>
@@ -1228,32 +1277,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -1264,16 +1313,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:6">
       <c r="F21" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
change add module name
</commit_message>
<xml_diff>
--- a/documents/projects_and_modules.xlsx
+++ b/documents/projects_and_modules.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Interfacing" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="Development Boards" sheetId="4" r:id="rId5"/>
     <sheet name=" Modules PCB " sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="108">
   <si>
     <t>ATMega 328</t>
   </si>
@@ -298,6 +298,51 @@
   </si>
   <si>
     <t>Servo Motor</t>
+  </si>
+  <si>
+    <t>4 channel relay board</t>
+  </si>
+  <si>
+    <t>4 digit seven segment display</t>
+  </si>
+  <si>
+    <t>adc module</t>
+  </si>
+  <si>
+    <t>avr programmer</t>
+  </si>
+  <si>
+    <t>dtmf module</t>
+  </si>
+  <si>
+    <t>rf module</t>
+  </si>
+  <si>
+    <t>keypad module</t>
+  </si>
+  <si>
+    <t>ldr module</t>
+  </si>
+  <si>
+    <t>motor driver</t>
+  </si>
+  <si>
+    <t>motor driver with ldr</t>
+  </si>
+  <si>
+    <t>rfid module</t>
+  </si>
+  <si>
+    <t>rs232 module</t>
+  </si>
+  <si>
+    <t>rtc module</t>
+  </si>
+  <si>
+    <t>dual channel relay driver</t>
+  </si>
+  <si>
+    <t>relay driver</t>
   </si>
 </sst>
 </file>
@@ -665,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -726,6 +771,7 @@
       <c r="A6" t="s">
         <v>17</v>
       </c>
+      <c r="B6" s="3"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4">
@@ -742,6 +788,7 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
@@ -971,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -998,31 +1045,39 @@
       <c r="A2" t="s">
         <v>29</v>
       </c>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>30</v>
       </c>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>41</v>
       </c>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>45</v>
       </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>46</v>
       </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>50</v>
       </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
@@ -1033,6 +1088,7 @@
       <c r="A9" t="s">
         <v>52</v>
       </c>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
@@ -1043,136 +1099,157 @@
       <c r="A11" t="s">
         <v>54</v>
       </c>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>55</v>
       </c>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>56</v>
       </c>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>57</v>
       </c>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>58</v>
       </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>86</v>
       </c>
+      <c r="B37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1316,14 +1393,92 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="F21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="21" spans="6:6">
       <c r="F21" t="s">
         <v>91</v>

</xml_diff>